<commit_message>
dashboard done,filedownload done,cleardb done
</commit_message>
<xml_diff>
--- a/filedownload/TemplateLoadExport.xlsx
+++ b/filedownload/TemplateLoadExport.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\prodigi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\prodigi\filedownload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C40FEC-4F49-4B3A-9D9B-F9A07AB359E6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="20490" windowHeight="7530" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="20490" windowHeight="7530" tabRatio="845"/>
   </bookViews>
   <sheets>
     <sheet name="BA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BA!$B$3:$V$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BA!$B$3:$V$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>PT. MEDIA MUSIK PROAKTIF</t>
   </si>
@@ -79,9 +78,6 @@
     <t xml:space="preserve">Rp </t>
   </si>
   <si>
-    <t>RP</t>
-  </si>
-  <si>
     <t>Rp</t>
   </si>
   <si>
@@ -94,9 +90,6 @@
     <t>Share Partner</t>
   </si>
   <si>
-    <t>Share Prodigi</t>
-  </si>
-  <si>
     <t>Revenue Artis</t>
   </si>
   <si>
@@ -106,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
@@ -228,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -297,21 +290,6 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -468,7 +446,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -501,9 +479,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -511,26 +491,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -539,7 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -548,7 +525,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -556,16 +533,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 11" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 12" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 15" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 19" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 20" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 10" xfId="2"/>
+    <cellStyle name="Normal 11" xfId="3"/>
+    <cellStyle name="Normal 12" xfId="4"/>
+    <cellStyle name="Normal 15" xfId="5"/>
+    <cellStyle name="Normal 19" xfId="6"/>
+    <cellStyle name="Normal 20" xfId="7"/>
+    <cellStyle name="Normal 3" xfId="8"/>
+    <cellStyle name="Normal 5" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -656,23 +633,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -708,23 +668,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -900,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:V153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1051,7 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>8</v>
@@ -1127,11 +1070,11 @@
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="31"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="17" t="s">
         <v>10</v>
       </c>
@@ -1145,11 +1088,11 @@
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="33" t="s">
-        <v>22</v>
+      <c r="D15" s="32" t="s">
+        <v>21</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
       <c r="G15" s="5"/>
       <c r="H15" s="21"/>
       <c r="I15" s="22" t="s">
@@ -1164,14 +1107,14 @@
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="33" t="s">
-        <v>23</v>
+      <c r="D16" s="25" t="s">
+        <v>22</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5"/>
       <c r="H16" s="21"/>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="28" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="19"/>
@@ -1180,18 +1123,18 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="26" t="s">
-        <v>24</v>
+      <c r="D17" s="32" t="s">
+        <v>23</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="5"/>
       <c r="H17" s="21"/>
-      <c r="I17" s="29" t="s">
-        <v>19</v>
+      <c r="I17" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="J17" s="19"/>
       <c r="K17" s="2"/>
@@ -1202,118 +1145,124 @@
     <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="19"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="2"/>
+      <c r="L18" s="15"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="20"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="15"/>
+      <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="25" t="s">
-        <v>19</v>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="24" t="s">
+        <v>18</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
-      <c r="V22" s="37"/>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+    </row>
+    <row r="23" spans="2:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -1325,33 +1274,26 @@
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
     </row>
-    <row r="24" spans="2:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="s">
-        <v>12</v>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>19</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1367,9 +1309,7 @@
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1416,36 +1356,36 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+    <row r="29" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="35"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="36"/>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -3420,34 +3360,17 @@
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
     </row>
-    <row r="154" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
-      <c r="J154" s="2"/>
-      <c r="K154" s="2"/>
-      <c r="L154" s="2"/>
-      <c r="M154" s="2"/>
-      <c r="N154" s="2"/>
-      <c r="O154" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B21:V21"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B22:V22"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B23:L23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TotalTrafic & TotalRevenue
</commit_message>
<xml_diff>
--- a/filedownload/TemplateLoadExport.xlsx
+++ b/filedownload/TemplateLoadExport.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>PT. MEDIA MUSIK PROAKTIF</t>
   </si>
@@ -118,22 +118,16 @@
     <t>Revenue Prodigi</t>
   </si>
   <si>
-    <t>SharePartner</t>
+    <t>Total trafic</t>
   </si>
   <si>
-    <t>Royalti Artis</t>
-  </si>
-  <si>
-    <t>Royalti Pencipta</t>
-  </si>
-  <si>
-    <t>ShareProdigi</t>
+    <t>total revenue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
@@ -541,6 +535,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,7 +575,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -1181,11 +1175,11 @@
     <row r="17" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="17" t="s">
         <v>10</v>
       </c>
@@ -1199,11 +1193,11 @@
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="5"/>
       <c r="H18" s="21"/>
       <c r="I18" s="22" t="s">
@@ -1237,11 +1231,11 @@
     <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="5"/>
       <c r="H20" s="21"/>
       <c r="I20" s="23" t="s">
@@ -1256,11 +1250,11 @@
     <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="5"/>
       <c r="H21" s="21"/>
       <c r="I21" s="23" t="s">
@@ -1275,11 +1269,11 @@
     <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="41"/>
       <c r="I22" s="6"/>
       <c r="J22" s="20"/>
       <c r="K22" s="2"/>
@@ -1332,29 +1326,29 @@
       <c r="V24" s="7"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="36"/>
-      <c r="U25" s="36"/>
-      <c r="V25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
@@ -1380,19 +1374,19 @@
       <c r="V26" s="7"/>
     </row>
     <row r="27" spans="2:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
@@ -1496,10 +1490,10 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="35" t="s">
+      <c r="I33" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J33" s="35"/>
+      <c r="J33" s="36"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -3511,10 +3505,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3522,57 +3516,44 @@
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="G1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="H1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="I1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="J1" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
connect all prodigi & proaktif
</commit_message>
<xml_diff>
--- a/filedownload/TemplateLoadExport.xlsx
+++ b/filedownload/TemplateLoadExport.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="20490" windowHeight="7530" tabRatio="845"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="20490" windowHeight="7530" tabRatio="845" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BA" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BA!$B$3:$V$34</definedName>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>PT. MEDIA MUSIK PROAKTIF</t>
   </si>
@@ -890,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:V157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -3508,7 +3512,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3558,5 +3562,242 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>